<commit_message>
Ajustes Filas rest controller
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/ejemplo1.xlsx
+++ b/src/main/resources/excel/ejemplo1.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="hojaejemplo1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="hojaejemplo2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="hojaejemplo3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="hojaejemplo11" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="hojaejemplo12" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="hojaejemplo13" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="5">
   <si>
     <t xml:space="preserve">a</t>
   </si>
@@ -111,8 +111,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -133,31 +137,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -177,36 +193,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -226,21 +257,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>